<commit_message>
changed the scope in pom.xml
</commit_message>
<xml_diff>
--- a/target/test-classes/testData/API_TestData.xlsx
+++ b/target/test-classes/testData/API_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F419869-5F47-4B7F-91BC-27F5DEA5877F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9769E484-899E-4743-B4CD-A173415A6628}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>testing@yahoo.co.in</t>
   </si>
@@ -70,10 +70,22 @@
     <t>job</t>
   </si>
   <si>
-    <t>Rahul Jha</t>
-  </si>
-  <si>
-    <t>Java Trainer</t>
+    <t>Rahul Arora</t>
+  </si>
+  <si>
+    <t>Selenium Master</t>
+  </si>
+  <si>
+    <t>Deepak</t>
+  </si>
+  <si>
+    <t>Ui Developer</t>
+  </si>
+  <si>
+    <t>Anil</t>
+  </si>
+  <si>
+    <t>Tech Lead</t>
   </si>
 </sst>
 </file>
@@ -425,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -525,6 +537,22 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>